<commit_message>
Internal version 1.1 Additional updates for TFS 1709.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34496
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="212">
   <si>
     <t>SourceID</t>
   </si>
@@ -416,9 +416,6 @@
     <t>('ManageCoachingLogs'),</t>
   </si>
   <si>
-    <t>('ManageWarningLogs')</t>
-  </si>
-  <si>
     <t xml:space="preserve"> INSERT INTO [EC].[AT_Action_Reasons]</t>
   </si>
   <si>
@@ -524,9 +521,6 @@
     <t xml:space="preserve">           ('WPPM13','Sr Analyst, Program',3,'Quality',1) </t>
   </si>
   <si>
-    <t xml:space="preserve">           </t>
-  </si>
-  <si>
     <t xml:space="preserve">            INSERT INTO [EC].[AT_Reassign_Status_For_Module]</t>
   </si>
   <si>
@@ -633,6 +627,42 @@
   </si>
   <si>
     <t>(103,203),</t>
+  </si>
+  <si>
+    <t>Additional updates. Admin Tool setup.</t>
+  </si>
+  <si>
+    <t>ReactivateCoachingLogs</t>
+  </si>
+  <si>
+    <t>ReactivateWarningLogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>('ManageWarningLogs'),</t>
+  </si>
+  <si>
+    <t>('ReactivateCoachingLogs'),</t>
+  </si>
+  <si>
+    <t>('ReactivateWarningLogs')</t>
+  </si>
+  <si>
+    <t>(103,205),</t>
+  </si>
+  <si>
+    <t>(101,206),</t>
+  </si>
+  <si>
+    <t>(103,207)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACS50','Manager, Customer Service',2,'Supervisor',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',1,'CSR',1)</t>
   </si>
 </sst>
 </file>
@@ -682,11 +712,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1032,10 +1063,27 @@
         <v>73</v>
       </c>
       <c r="D2">
-        <v>709</v>
+        <v>1709</v>
       </c>
       <c r="E2" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3">
+        <v>1709</v>
+      </c>
+      <c r="E3" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1207,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1167,9 +1215,10 @@
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>88</v>
       </c>
@@ -1180,7 +1229,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>201</v>
       </c>
@@ -1191,7 +1240,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>202</v>
       </c>
@@ -1201,8 +1250,11 @@
       <c r="F3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>203</v>
       </c>
@@ -1213,7 +1265,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>204</v>
       </c>
@@ -1224,7 +1276,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>205</v>
       </c>
@@ -1235,14 +1287,36 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
       <c r="F7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>202</v>
+      </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1326,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1260,6 +1334,7 @@
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1269,6 +1344,9 @@
       <c r="B1" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="F1" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1278,7 +1356,7 @@
         <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,7 +1367,7 @@
         <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1300,7 +1378,7 @@
         <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,18 +1389,18 @@
         <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1330,10 +1408,10 @@
         <v>102</v>
       </c>
       <c r="B7">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,21 +1419,21 @@
         <v>102</v>
       </c>
       <c r="B8">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1363,10 +1441,10 @@
         <v>103</v>
       </c>
       <c r="B10">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1374,29 +1452,47 @@
         <v>103</v>
       </c>
       <c r="B11">
+        <v>203</v>
+      </c>
+      <c r="F11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>103</v>
+      </c>
+      <c r="B12">
         <v>205</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>200</v>
-      </c>
-    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>103</v>
+      </c>
+      <c r="B13">
+        <v>207</v>
+      </c>
       <c r="F13" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="3">
-        <v>-103205</v>
+      <c r="F14" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1443,7 +1539,7 @@
         <v>99</v>
       </c>
       <c r="M1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1472,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1501,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1530,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1559,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1588,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1617,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1646,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1675,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1704,47 +1800,47 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1754,7 +1850,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1765,6 +1861,7 @@
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="101.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1784,7 +1881,7 @@
         <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1804,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1824,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1844,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1864,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1884,7 +1981,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1904,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1924,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1944,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1984,42 +2081,77 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>163</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>165</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2093,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2113,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2133,7 +2265,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2153,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2173,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2193,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2213,52 +2345,52 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2296,13 +2428,13 @@
         <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2325,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2348,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2371,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2394,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2417,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2440,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2463,42 +2595,42 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 2.0. TFS 3416
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34782
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="213">
   <si>
     <t>SourceID</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Sr Manager, Customer Service</t>
   </si>
   <si>
-    <t>WISY13</t>
-  </si>
-  <si>
     <t>Sr Analyst, Systems</t>
   </si>
   <si>
@@ -491,21 +488,6 @@
     <t xml:space="preserve">              VALUES</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',1,'CSR',1),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',2,'Supervisor',1),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',3,'Quality',1),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',4,'LSA',1),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',5,'Training',1),</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WACS50','Manager, Customer Service',1,'CSR',1),</t>
   </si>
   <si>
@@ -575,9 +557,6 @@
     <t xml:space="preserve">           ,[AddToUser]</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',101,'CoachingAdmin',0,1),</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WACS50','Manager, Customer Service',102,'CoachingUser',1,1),</t>
   </si>
   <si>
@@ -593,9 +572,6 @@
     <t xml:space="preserve">           ('WPPM13','Sr Analyst, Program',102,'CoachingUser',1,1),</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WISY13','Sr Analyst, Systems',103,'WarningAdmin',0,1)</t>
-  </si>
-  <si>
     <t>INSERT INTO [EC].[AT_Role_Entitlement_Link]</t>
   </si>
   <si>
@@ -663,6 +639,33 @@
   </si>
   <si>
     <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',1,'CSR',1)</t>
+  </si>
+  <si>
+    <t>Replace jobcode WISY13 with WISY14</t>
+  </si>
+  <si>
+    <t>WISY14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',1,'CSR',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',2,'Supervisor',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',3,'Quality',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',4,'LSA',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',5,'Training',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',103,'WarningAdmin',0,1)</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1025,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1037,19 +1040,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1060,13 +1063,13 @@
         <v>42503</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>1709</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,13 +1080,30 @@
         <v>42515</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>1709</v>
       </c>
       <c r="E3" t="s">
-        <v>200</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42577</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <v>3416</v>
+      </c>
+      <c r="E4" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1107,16 +1127,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1124,13 +1144,13 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,13 +1158,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,13 +1172,13 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1166,38 +1186,38 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1220,13 +1240,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1234,10 +1254,10 @@
         <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,13 +1265,13 @@
         <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1259,10 +1279,10 @@
         <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1270,10 +1290,10 @@
         <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1281,10 +1301,10 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1292,10 +1312,10 @@
         <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1303,20 +1323,20 @@
         <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F8" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1339,13 +1359,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1356,7 +1376,7 @@
         <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1367,7 +1387,7 @@
         <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1378,7 +1398,7 @@
         <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,7 +1409,7 @@
         <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,7 +1420,7 @@
         <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1411,7 +1431,7 @@
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1422,7 +1442,7 @@
         <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1433,7 +1453,7 @@
         <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1444,7 +1464,7 @@
         <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1455,7 +1475,7 @@
         <v>203</v>
       </c>
       <c r="F11" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1466,7 +1486,7 @@
         <v>205</v>
       </c>
       <c r="F12" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1477,17 +1497,17 @@
         <v>207</v>
       </c>
       <c r="F13" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F14" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F15" s="4" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1515,10 +1535,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>53</v>
@@ -1527,19 +1547,19 @@
         <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="M1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1547,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1568,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1576,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1597,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1605,7 +1625,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1626,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1655,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1663,7 +1683,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1684,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1692,7 +1712,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1713,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1721,7 +1741,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1742,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1750,7 +1770,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1771,7 +1791,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1779,7 +1799,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1800,47 +1820,47 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1866,13 +1888,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>58</v>
@@ -1881,15 +1903,15 @@
         <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1901,15 +1923,15 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1921,15 +1943,15 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1941,47 +1963,47 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2001,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2021,55 +2043,55 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
         <v>77</v>
-      </c>
-      <c r="B9" t="s">
-        <v>78</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
         <v>67</v>
-      </c>
-      <c r="B10" t="s">
-        <v>68</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2081,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>157</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2101,7 +2123,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2121,37 +2143,37 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2176,13 +2198,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
@@ -2225,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2245,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2259,13 +2281,13 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2285,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2293,7 +2315,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -2305,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2313,7 +2335,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -2325,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2333,7 +2355,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -2345,52 +2367,52 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2416,39 +2440,39 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
       </c>
       <c r="C2">
         <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2457,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2471,7 +2495,7 @@
         <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2480,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2494,7 +2518,7 @@
         <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2503,21 +2527,21 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
         <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>78</v>
       </c>
       <c r="C5">
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2526,21 +2550,21 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
       </c>
       <c r="C6">
         <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2549,21 +2573,21 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
         <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
       </c>
       <c r="C7">
         <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2572,21 +2596,21 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
       </c>
       <c r="C8">
         <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2595,42 +2619,42 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K12" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for TFS 3877.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C35294
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" tabRatio="596"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="218">
   <si>
     <t>SourceID</t>
   </si>
@@ -665,7 +665,22 @@
     <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',101,'CoachingAdmin',0,1),</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',103,'WarningAdmin',0,1)</t>
+    <t>Add jobcode WACQ13 in Role_access table(Mark Hackman and Scott Potter)</t>
+  </si>
+  <si>
+    <t>WACQ13</t>
+  </si>
+  <si>
+    <t>Sr Specialist, Quality (CS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',103,'WarningAdmin',0,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',103,'WarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      ('WACQ13','Sr Specialist, Quality (CS)',101,'CoachingAdmin',0,1),</t>
   </si>
 </sst>
 </file>
@@ -1025,20 +1040,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="144.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="144.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>69</v>
       </c>
@@ -1055,7 +1072,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1072,7 +1089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -1089,7 +1106,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1104,6 +1121,23 @@
       </c>
       <c r="E4" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42633</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>3877</v>
+      </c>
+      <c r="E5" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1118,14 +1152,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -1139,7 +1173,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1153,7 +1187,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -1167,7 +1201,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -1181,7 +1215,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1195,27 +1229,27 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>120</v>
       </c>
@@ -1231,14 +1265,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -1249,7 +1283,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201</v>
       </c>
@@ -1260,7 +1294,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>202</v>
       </c>
@@ -1274,7 +1308,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>203</v>
       </c>
@@ -1285,7 +1319,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>204</v>
       </c>
@@ -1296,7 +1330,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>205</v>
       </c>
@@ -1307,7 +1341,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>206</v>
       </c>
@@ -1318,7 +1352,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>207</v>
       </c>
@@ -1329,12 +1363,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>198</v>
       </c>
@@ -1350,14 +1384,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -1368,7 +1402,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1379,7 +1413,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
@@ -1390,7 +1424,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>101</v>
       </c>
@@ -1401,7 +1435,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>101</v>
       </c>
@@ -1412,7 +1446,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>101</v>
       </c>
@@ -1423,7 +1457,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>102</v>
       </c>
@@ -1434,7 +1468,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>102</v>
       </c>
@@ -1445,7 +1479,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>102</v>
       </c>
@@ -1456,7 +1490,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>103</v>
       </c>
@@ -1467,7 +1501,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>103</v>
       </c>
@@ -1478,7 +1512,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>103</v>
       </c>
@@ -1489,7 +1523,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>103</v>
       </c>
@@ -1500,12 +1534,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F14" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F15" s="4" t="s">
         <v>201</v>
       </c>
@@ -1522,18 +1556,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>94</v>
       </c>
@@ -1562,7 +1596,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1591,7 +1625,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1620,7 +1654,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1649,7 +1683,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1678,7 +1712,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1707,7 +1741,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1736,7 +1770,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1765,7 +1799,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1794,7 +1828,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1823,42 +1857,42 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M13" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M18" t="s">
         <v>145</v>
       </c>
@@ -1876,17 +1910,17 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="101.42578125" customWidth="1"/>
+    <col min="9" max="9" width="101.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -1906,7 +1940,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -1926,7 +1960,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -1946,7 +1980,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -1966,7 +2000,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>205</v>
       </c>
@@ -1986,7 +2020,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>205</v>
       </c>
@@ -2006,7 +2040,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2026,7 +2060,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -2046,7 +2080,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -2066,7 +2100,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2086,7 +2120,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -2106,7 +2140,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2126,7 +2160,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2146,32 +2180,32 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I15" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
         <v>157</v>
       </c>
@@ -2187,16 +2221,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
@@ -2213,7 +2247,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2230,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2250,7 +2284,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2270,7 +2304,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2290,7 +2324,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2310,7 +2344,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2330,7 +2364,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2350,7 +2384,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2370,47 +2404,47 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
         <v>169</v>
       </c>
@@ -2422,23 +2456,23 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -2461,7 +2495,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -2484,7 +2518,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -2507,7 +2541,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2530,7 +2564,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -2553,7 +2587,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2576,7 +2610,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2599,7 +2633,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -2622,39 +2656,85 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
       <c r="K9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10">
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
       <c r="K10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
-        <v>212</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2668,14 +2748,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2686,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2697,7 +2777,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2708,7 +2788,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2719,7 +2799,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2730,7 +2810,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2741,7 +2821,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2752,7 +2832,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2763,7 +2843,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2774,7 +2854,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2785,7 +2865,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2796,7 +2876,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2807,7 +2887,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2818,7 +2898,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2829,7 +2909,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2840,7 +2920,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2851,7 +2931,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2862,7 +2942,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2873,7 +2953,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2884,7 +2964,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2895,7 +2975,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2906,7 +2986,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2917,7 +2997,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2928,7 +3008,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2939,7 +3019,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2950,7 +3030,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2961,7 +3041,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2972,7 +3052,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2983,7 +3063,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2994,7 +3074,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -3005,7 +3085,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -3016,7 +3096,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -3027,7 +3107,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -3038,7 +3118,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -3049,7 +3129,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -3060,7 +3140,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -3071,7 +3151,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -3082,7 +3162,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -3093,7 +3173,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -3104,7 +3184,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -3115,7 +3195,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -3126,7 +3206,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -3137,7 +3217,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -3148,7 +3228,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -3159,7 +3239,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -3170,7 +3250,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -3181,7 +3261,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -3192,7 +3272,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updates for TFS 3027.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C36039
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="222">
   <si>
     <t>SourceID</t>
   </si>
@@ -681,6 +681,18 @@
   </si>
   <si>
     <t xml:space="preserve">      ('WACQ13','Sr Specialist, Quality (CS)',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t>SeniorManager</t>
+  </si>
+  <si>
+    <t>SeniorManagerDashboard</t>
+  </si>
+  <si>
+    <t>Principal Analyst, Systems</t>
+  </si>
+  <si>
+    <t>Adding rows for SrMgr Dashboard support(Role, Entitlement, Role_Entitlement Link, Role Access Tables</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,6 +1152,23 @@
         <v>212</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42691</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>3027</v>
+      </c>
+      <c r="E6" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1150,7 +1179,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1230,6 +1261,15 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="F6" t="s">
         <v>116</v>
       </c>
@@ -1263,7 +1303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1364,6 +1406,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
       <c r="F9" t="s">
         <v>197</v>
       </c>
@@ -1382,7 +1430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1535,6 +1585,12 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <v>208</v>
+      </c>
       <c r="F14" s="3" t="s">
         <v>200</v>
       </c>
@@ -2459,7 +2515,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2500,7 +2556,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -2520,19 +2576,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="C3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2543,10 +2599,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>102</v>
@@ -2566,10 +2622,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>102</v>
@@ -2589,10 +2645,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C6">
         <v>102</v>
@@ -2612,10 +2668,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C7">
         <v>102</v>
@@ -2635,19 +2691,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C8">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2658,16 +2714,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C9">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2703,6 +2759,24 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="K11" t="s">
         <v>177</v>
       </c>

</xml_diff>